<commit_message>
BOM & Pics Updates
</commit_message>
<xml_diff>
--- a/Bill of Materials BOM/BOM.xlsx
+++ b/Bill of Materials BOM/BOM.xlsx
@@ -1,20 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
-  <workbookProtection/>
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+  <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="16380" windowHeight="8190" tabRatio="500"/>
   </bookViews>
   <sheets>
-    <sheet name="Air Unit" sheetId="1" state="visible" r:id="rId2"/>
-    <sheet name="Ground Unit" sheetId="2" state="visible" r:id="rId3"/>
-    <sheet name="Optional Extras" sheetId="3" state="visible" r:id="rId4"/>
-    <sheet name="Nano Talon UAV" sheetId="4" state="visible" r:id="rId5"/>
-    <sheet name="Sheet5" sheetId="5" state="visible" r:id="rId6"/>
+    <sheet name="Air Unit" sheetId="1" r:id="rId1"/>
+    <sheet name="Ground Unit" sheetId="2" r:id="rId2"/>
+    <sheet name="Optional Extras" sheetId="3" r:id="rId3"/>
+    <sheet name="Nano Talon UAV" sheetId="4" r:id="rId4"/>
+    <sheet name="Sheet5" sheetId="5" r:id="rId5"/>
   </sheets>
-  <calcPr iterateCount="100" refMode="A1" iterate="false" iterateDelta="0.001"/>
+  <calcPr calcId="125725"/>
   <extLst>
     <ext xmlns:loext="http://schemas.libreoffice.org/" uri="{7626C862-2A13-11E5-B345-FEFF819CDC9F}">
       <loext:extCalcPr stringRefSyntax="CalcA1ExcelA1"/>
@@ -24,9 +23,9 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="50">
-  <si>
-    <t xml:space="preserve">Bill of Materials (BOM):</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="101" uniqueCount="49">
+  <si>
+    <t>Bill of Materials (BOM):</t>
   </si>
   <si>
     <t xml:space="preserve"> Component </t>
@@ -35,13 +34,13 @@
     <t xml:space="preserve"> Source  to Buy them</t>
   </si>
   <si>
-    <t xml:space="preserve">Price</t>
+    <t>Price</t>
   </si>
   <si>
     <t xml:space="preserve">Notes: </t>
   </si>
   <si>
-    <t xml:space="preserve">Total Cost USD</t>
+    <t>Total Cost USD</t>
   </si>
   <si>
     <t xml:space="preserve">D1 Mini Pro </t>
@@ -50,85 +49,85 @@
     <t xml:space="preserve"> https://amzn.to/2ZQArbl</t>
   </si>
   <si>
-    <t xml:space="preserve">With antenna included</t>
+    <t>With antenna included</t>
   </si>
   <si>
     <t xml:space="preserve"> https://amzn.to/2ZNQEy1</t>
   </si>
   <si>
-    <t xml:space="preserve">Circuit Board (PCB)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">http://store.mkme.org/product/resq-printed-circuit-board-v1-1/</t>
-  </si>
-  <si>
-    <t xml:space="preserve">SD Card Reader</t>
+    <t>Circuit Board (PCB)</t>
+  </si>
+  <si>
+    <t>http://store.mkme.org/product/resq-printed-circuit-board-v1-1/</t>
+  </si>
+  <si>
+    <t>SD Card Reader</t>
   </si>
   <si>
     <t xml:space="preserve"> https://amzn.to/2XPDv6B</t>
   </si>
   <si>
-    <t xml:space="preserve">0.96" OLED Display</t>
+    <t>0.96" OLED Display</t>
   </si>
   <si>
     <t xml:space="preserve"> https://amzn.to/3cCHvvj</t>
   </si>
   <si>
-    <t xml:space="preserve">V1.1 PCB Files VCC at end V2.1 Ground at End</t>
-  </si>
-  <si>
-    <t xml:space="preserve">2.4 GHz Yagi Antenna</t>
+    <t>V1.1 PCB Files VCC at end V2.1 Ground at End</t>
+  </si>
+  <si>
+    <t>2.4 GHz Yagi Antenna</t>
   </si>
   <si>
     <t xml:space="preserve"> https://amzn.to/3gwLso9</t>
   </si>
   <si>
-    <t xml:space="preserve">BN220 GPS</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://amzn.to/3fYKhfO</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Servo Wire For VCC from FC</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://amzn.to/3kI5BcL</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Micro SD Card</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://amzn.to/2FjEO6y</t>
+    <t>BN220 GPS</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3fYKhfO</t>
+  </si>
+  <si>
+    <t>Servo Wire For VCC from FC</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3kI5BcL</t>
+  </si>
+  <si>
+    <t>Micro SD Card</t>
+  </si>
+  <si>
+    <t>https://amzn.to/2FjEO6y</t>
   </si>
   <si>
     <t xml:space="preserve">Total Cost USD </t>
   </si>
   <si>
-    <t xml:space="preserve">Lipo Battery 200mah</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://amzn.to/33VoPFN</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Adafruit Power Boost Charger</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://amzn.to/3aknA4a</t>
+    <t>Lipo Battery 200mah</t>
+  </si>
+  <si>
+    <t>https://amzn.to/33VoPFN</t>
+  </si>
+  <si>
+    <t>Adafruit Power Boost Charger</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3aknA4a</t>
   </si>
   <si>
     <t xml:space="preserve">Total Cost: </t>
   </si>
   <si>
-    <t xml:space="preserve">SMA adapter</t>
+    <t>SMA adapter</t>
   </si>
   <si>
     <t xml:space="preserve"> https://amzn.to/3ezOpT8</t>
   </si>
   <si>
-    <t xml:space="preserve">Spare for UFLs that can get damaged</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nrf24l01</t>
+    <t>Spare for UFLs that can get damaged</t>
+  </si>
+  <si>
+    <t>nrf24l01</t>
   </si>
   <si>
     <t xml:space="preserve"> https://amzn.to/3exhePP</t>
@@ -137,34 +136,31 @@
     <t xml:space="preserve">Use this for extra telemetry instead of 3DR I used </t>
   </si>
   <si>
-    <t xml:space="preserve">LORA Modules</t>
+    <t>LORA Modules</t>
   </si>
   <si>
     <t xml:space="preserve"> https://amzn.to/2zB61ze</t>
   </si>
   <si>
-    <t xml:space="preserve">LiOn 5200mAh</t>
-  </si>
-  <si>
-    <t xml:space="preserve">https://amzn.to/3kJbMO2</t>
-  </si>
-  <si>
-    <t xml:space="preserve">Lithium Ion HUUUUGE capacity but needs a diff charge control</t>
-  </si>
-  <si>
-    <t xml:space="preserve">LNA</t>
+    <t>LiOn 5200mAh</t>
+  </si>
+  <si>
+    <t>https://amzn.to/3kJbMO2</t>
+  </si>
+  <si>
+    <t>Lithium Ion HUUUUGE capacity but needs a diff charge control</t>
   </si>
   <si>
     <t xml:space="preserve">Total Cost USD : </t>
   </si>
   <si>
-    <t xml:space="preserve">Nano Talon PNP Aircraft</t>
+    <t>Nano Talon PNP Aircraft</t>
   </si>
   <si>
     <t xml:space="preserve"> https://www.banggood.com/ZOHD-Nano-Talon-860mm-Wingspan-AIO-HD-V-Tail-EPP-FPV-RC-Airplane-PNP-With-Gyro-p-1168297.html?rmmds=search&amp;p=S808226360906201609Z&amp;custlinkid=482321&amp;cur_warehouse=CN</t>
   </si>
   <si>
-    <t xml:space="preserve">F722 Wing Flight Controller</t>
+    <t>F722 Wing Flight Controller</t>
   </si>
   <si>
     <t xml:space="preserve"> https://amzn.to/2ZSoMsz</t>
@@ -173,18 +169,17 @@
     <t xml:space="preserve">18650 LiOn cells </t>
   </si>
   <si>
-    <t xml:space="preserve">Ill finish this another day. Im done</t>
+    <t>Ill finish this another day. Im done</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="2">
-    <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="[$$-1009]#,##0.00;[RED]\-[$$-1009]#,##0.00"/>
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="[$$-1009]#,##0.00;[Red]\-[$$-1009]#,##0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="4">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -192,30 +187,15 @@
       <charset val="1"/>
     </font>
     <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <name val="Arial"/>
-      <family val="0"/>
-    </font>
-    <font>
-      <b val="true"/>
+      <b/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
       <charset val="1"/>
     </font>
     <font>
-      <b val="true"/>
-      <u val="single"/>
+      <b/>
+      <u/>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
@@ -250,7 +230,7 @@
     </fill>
   </fills>
   <borders count="1">
-    <border diagonalUp="false" diagonalDown="false">
+    <border>
       <left/>
       <right/>
       <top/>
@@ -258,89 +238,50 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="20">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="true" applyAlignment="true" applyProtection="true">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
-    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
+  <cellStyleXfs count="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="12">
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="5" fillId="3" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="2" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="2" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="left" vertical="top" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
-    </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="general" vertical="top" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
-      <protection locked="true" hidden="false"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="top"/>
     </xf>
   </cellXfs>
-  <cellStyles count="6">
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
-    <cellStyle name="Comma" xfId="15" builtinId="3"/>
-    <cellStyle name="Comma [0]" xfId="16" builtinId="6"/>
-    <cellStyle name="Currency" xfId="17" builtinId="4"/>
-    <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
-    <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
+  <dxfs count="0"/>
+  <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -399,40 +340,328 @@
       <rgbColor rgb="FF993366"/>
       <rgbColor rgb="FF333399"/>
       <rgbColor rgb="FF333333"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
     </indexedColors>
   </colors>
 </styleSheet>
 </file>
 
+<file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+  <a:themeElements>
+    <a:clrScheme name="Office">
+      <a:dk1>
+        <a:sysClr val="windowText" lastClr="000000"/>
+      </a:dk1>
+      <a:lt1>
+        <a:sysClr val="window" lastClr="FFFFFF"/>
+      </a:lt1>
+      <a:dk2>
+        <a:srgbClr val="1F497D"/>
+      </a:dk2>
+      <a:lt2>
+        <a:srgbClr val="EEECE1"/>
+      </a:lt2>
+      <a:accent1>
+        <a:srgbClr val="4F81BD"/>
+      </a:accent1>
+      <a:accent2>
+        <a:srgbClr val="C0504D"/>
+      </a:accent2>
+      <a:accent3>
+        <a:srgbClr val="9BBB59"/>
+      </a:accent3>
+      <a:accent4>
+        <a:srgbClr val="8064A2"/>
+      </a:accent4>
+      <a:accent5>
+        <a:srgbClr val="4BACC6"/>
+      </a:accent5>
+      <a:accent6>
+        <a:srgbClr val="F79646"/>
+      </a:accent6>
+      <a:hlink>
+        <a:srgbClr val="0000FF"/>
+      </a:hlink>
+      <a:folHlink>
+        <a:srgbClr val="800080"/>
+      </a:folHlink>
+    </a:clrScheme>
+    <a:fontScheme name="Office">
+      <a:majorFont>
+        <a:latin typeface="Cambria"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Times New Roman"/>
+        <a:font script="Hebr" typeface="Times New Roman"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="MoolBoran"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Times New Roman"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:majorFont>
+      <a:minorFont>
+        <a:latin typeface="Calibri"/>
+        <a:ea typeface=""/>
+        <a:cs typeface=""/>
+        <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
+        <a:font script="Hang" typeface="맑은 고딕"/>
+        <a:font script="Hans" typeface="宋体"/>
+        <a:font script="Hant" typeface="新細明體"/>
+        <a:font script="Arab" typeface="Arial"/>
+        <a:font script="Hebr" typeface="Arial"/>
+        <a:font script="Thai" typeface="Tahoma"/>
+        <a:font script="Ethi" typeface="Nyala"/>
+        <a:font script="Beng" typeface="Vrinda"/>
+        <a:font script="Gujr" typeface="Shruti"/>
+        <a:font script="Khmr" typeface="DaunPenh"/>
+        <a:font script="Knda" typeface="Tunga"/>
+        <a:font script="Guru" typeface="Raavi"/>
+        <a:font script="Cans" typeface="Euphemia"/>
+        <a:font script="Cher" typeface="Plantagenet Cherokee"/>
+        <a:font script="Yiii" typeface="Microsoft Yi Baiti"/>
+        <a:font script="Tibt" typeface="Microsoft Himalaya"/>
+        <a:font script="Thaa" typeface="MV Boli"/>
+        <a:font script="Deva" typeface="Mangal"/>
+        <a:font script="Telu" typeface="Gautami"/>
+        <a:font script="Taml" typeface="Latha"/>
+        <a:font script="Syrc" typeface="Estrangelo Edessa"/>
+        <a:font script="Orya" typeface="Kalinga"/>
+        <a:font script="Mlym" typeface="Kartika"/>
+        <a:font script="Laoo" typeface="DokChampa"/>
+        <a:font script="Sinh" typeface="Iskoola Pota"/>
+        <a:font script="Mong" typeface="Mongolian Baiti"/>
+        <a:font script="Viet" typeface="Arial"/>
+        <a:font script="Uigh" typeface="Microsoft Uighur"/>
+      </a:minorFont>
+    </a:fontScheme>
+    <a:fmtScheme name="Office">
+      <a:fillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="50000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="35000">
+              <a:schemeClr val="phClr">
+                <a:tint val="37000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:tint val="15000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="1"/>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:shade val="51000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="80000">
+              <a:schemeClr val="phClr">
+                <a:shade val="93000"/>
+                <a:satMod val="130000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="94000"/>
+                <a:satMod val="135000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:lin ang="16200000" scaled="0"/>
+        </a:gradFill>
+      </a:fillStyleLst>
+      <a:lnStyleLst>
+        <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr">
+              <a:shade val="95000"/>
+              <a:satMod val="105000"/>
+            </a:schemeClr>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="25400" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+        <a:ln w="38100" cap="flat" cmpd="sng" algn="ctr">
+          <a:solidFill>
+            <a:schemeClr val="phClr"/>
+          </a:solidFill>
+          <a:prstDash val="solid"/>
+        </a:ln>
+      </a:lnStyleLst>
+      <a:effectStyleLst>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="20000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="38000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+        </a:effectStyle>
+        <a:effectStyle>
+          <a:effectLst>
+            <a:outerShdw blurRad="40000" dist="23000" dir="5400000" rotWithShape="0">
+              <a:srgbClr val="000000">
+                <a:alpha val="35000"/>
+              </a:srgbClr>
+            </a:outerShdw>
+          </a:effectLst>
+          <a:scene3d>
+            <a:camera prst="orthographicFront">
+              <a:rot lat="0" lon="0" rev="0"/>
+            </a:camera>
+            <a:lightRig rig="threePt" dir="t">
+              <a:rot lat="0" lon="0" rev="1200000"/>
+            </a:lightRig>
+          </a:scene3d>
+          <a:sp3d>
+            <a:bevelT w="63500" h="25400"/>
+          </a:sp3d>
+        </a:effectStyle>
+      </a:effectStyleLst>
+      <a:bgFillStyleLst>
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="40000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="40000">
+              <a:schemeClr val="phClr">
+                <a:tint val="45000"/>
+                <a:shade val="99000"/>
+                <a:satMod val="350000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="20000"/>
+                <a:satMod val="255000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="-80000" r="50000" b="180000"/>
+          </a:path>
+        </a:gradFill>
+        <a:gradFill rotWithShape="1">
+          <a:gsLst>
+            <a:gs pos="0">
+              <a:schemeClr val="phClr">
+                <a:tint val="80000"/>
+                <a:satMod val="300000"/>
+              </a:schemeClr>
+            </a:gs>
+            <a:gs pos="100000">
+              <a:schemeClr val="phClr">
+                <a:shade val="30000"/>
+                <a:satMod val="200000"/>
+              </a:schemeClr>
+            </a:gs>
+          </a:gsLst>
+          <a:path path="circle">
+            <a:fillToRect l="50000" t="50000" r="50000" b="50000"/>
+          </a:path>
+        </a:gradFill>
+      </a:bgFillStyleLst>
+    </a:fmtScheme>
+  </a:themeElements>
+  <a:objectDefaults/>
+  <a:extraClrSchemeLst/>
+</a:theme>
+</file>
+
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:AMK16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A22" activeCellId="0" sqref="A22"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="26.53"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="38.33"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="44.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="14.62"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.54"/>
+    <col min="1" max="1" width="26.5703125" style="1" customWidth="1"/>
+    <col min="2" max="2" width="38.28515625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="44.7109375" style="1" customWidth="1"/>
+    <col min="5" max="5" width="14.5703125" style="1" customWidth="1"/>
+    <col min="6" max="1025" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="22.15" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -448,141 +677,140 @@
       <c r="E2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="8" t="n">
-        <f aca="false">SUM(C3:C99)</f>
-        <v>93.69</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="8">
+        <f>SUM(C3:C99)</f>
+        <v>96.69</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="9">
         <v>7.99</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="9">
         <v>7.99</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6" ht="25.5">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="9">
         <v>7.99</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="9">
         <v>6.99</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="9">
         <v>22.45</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="9">
         <v>15.99</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
         <v>21</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="9">
         <v>7</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="9">
         <v>10.29</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="https://amzn.to/3fYKhfO"/>
+    <hyperlink ref="B10" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.025" bottom="1.025" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.0249999999999999" bottom="1.0249999999999999" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup orientation="portrait" useFirstPageNumber="1" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;A</oddHeader>
     <oddFooter>&amp;CPage &amp;P</oddFooter>
   </headerFooter>
@@ -591,33 +819,30 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:AMK16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="C7" sqref="C7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="61.4"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="41.8"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="16.24"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.54"/>
+    <col min="1" max="1" width="25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="61.42578125" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="41.85546875" style="1" customWidth="1"/>
+    <col min="5" max="5" width="16.28515625" style="1" customWidth="1"/>
+    <col min="6" max="1025" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="22.15" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -633,148 +858,147 @@
       <c r="E2" s="7" t="s">
         <v>25</v>
       </c>
-      <c r="F2" s="8" t="n">
-        <f aca="false">SUM(C3:C99)</f>
-        <v>116.67</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="8">
+        <f>SUM(C3:C99)</f>
+        <v>119.66999999999999</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="C4" s="9" t="n">
+      <c r="C4" s="9">
         <v>7.99</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>8</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="C5" s="9" t="n">
+      <c r="C5" s="9">
         <v>7.99</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6">
       <c r="A6" s="1" t="s">
         <v>10</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="9" t="n">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="C6" s="9">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6">
       <c r="A7" s="1" t="s">
         <v>12</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>13</v>
       </c>
-      <c r="C7" s="9" t="n">
+      <c r="C7" s="9">
         <v>7.99</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6">
       <c r="A8" s="1" t="s">
         <v>14</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>15</v>
       </c>
-      <c r="C8" s="9" t="n">
+      <c r="C8" s="9">
         <v>6.99</v>
       </c>
       <c r="D8" s="1" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:6">
       <c r="A9" s="1" t="s">
         <v>17</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>18</v>
       </c>
-      <c r="C9" s="9" t="n">
+      <c r="C9" s="9">
         <v>22.45</v>
       </c>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6">
       <c r="A10" s="1" t="s">
         <v>19</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="C10" s="9" t="n">
+      <c r="C10" s="9">
         <v>15.99</v>
       </c>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6">
       <c r="A11" s="11" t="s">
         <v>23</v>
       </c>
       <c r="B11" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="C11" s="9" t="n">
+      <c r="C11" s="9">
         <v>10.29</v>
       </c>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6">
       <c r="A12" s="11" t="s">
         <v>26</v>
       </c>
       <c r="B12" s="11" t="s">
         <v>27</v>
       </c>
-      <c r="C12" s="9" t="n">
+      <c r="C12" s="9">
         <v>14.99</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6">
       <c r="A13" s="11" t="s">
         <v>28</v>
       </c>
       <c r="B13" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C13" s="9" t="n">
+      <c r="C13" s="9">
         <v>14.99</v>
       </c>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="B10" r:id="rId1" display="https://amzn.to/3fYKhfO"/>
+    <hyperlink ref="B10" r:id="rId1"/>
   </hyperlinks>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -783,33 +1007,30 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:AMK15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="A9" sqref="A9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="36.82"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="44.72"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="13.21"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.54"/>
+    <col min="1" max="1" width="25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="36.85546875" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="74.28515625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="13.140625" style="1" customWidth="1"/>
+    <col min="6" max="1025" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="22.15" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -825,19 +1046,19 @@
       <c r="E2" s="7" t="s">
         <v>30</v>
       </c>
-      <c r="F2" s="8" t="n">
-        <f aca="false">SUM(C3:C98)</f>
-        <v>29.98</v>
-      </c>
-    </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="F2" s="8">
+        <f>SUM(C3:C98)</f>
+        <v>29.979999999999997</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
       <c r="A3" s="1" t="s">
         <v>31</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>32</v>
       </c>
-      <c r="C3" s="1" t="n">
+      <c r="C3" s="1">
         <v>3.99</v>
       </c>
       <c r="D3" s="1" t="s">
@@ -846,7 +1067,7 @@
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6">
       <c r="A4" s="1" t="s">
         <v>34</v>
       </c>
@@ -858,7 +1079,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="5" spans="1:6">
       <c r="A5" s="1" t="s">
         <v>37</v>
       </c>
@@ -870,61 +1091,57 @@
         <v>36</v>
       </c>
     </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="6" spans="1:6">
       <c r="A6" s="11" t="s">
         <v>39</v>
       </c>
       <c r="B6" s="11" t="s">
         <v>40</v>
       </c>
-      <c r="C6" s="9" t="n">
+      <c r="C6" s="9">
         <v>25.99</v>
       </c>
       <c r="D6" s="1" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:6">
       <c r="C7" s="9"/>
     </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:6">
       <c r="C8" s="9"/>
     </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="1" t="s">
-        <v>42</v>
-      </c>
+    <row r="9" spans="1:6">
       <c r="C9" s="9"/>
     </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="10" spans="1:6">
       <c r="A10" s="11"/>
       <c r="B10" s="11"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -933,33 +1150,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
-  <dimension ref="A1:F16"/>
+  <dimension ref="A1:AMK16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="D2" sqref="D2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.01"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="2" width="68.66"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="13.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="25.12"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="15.8"/>
-    <col collapsed="false" customWidth="false" hidden="false" outlineLevel="0" max="1025" min="6" style="1" width="11.54"/>
+    <col min="1" max="1" width="25" style="1" customWidth="1"/>
+    <col min="2" max="2" width="68.7109375" style="2" customWidth="1"/>
+    <col min="3" max="3" width="13.42578125" style="1" customWidth="1"/>
+    <col min="4" max="4" width="25.140625" style="1" customWidth="1"/>
+    <col min="5" max="5" width="15.85546875" style="1" customWidth="1"/>
+    <col min="6" max="1025" width="11.5703125" style="1"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="22.2" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:6" ht="22.15" customHeight="1">
       <c r="A1" s="3" t="s">
         <v>0</v>
       </c>
       <c r="E1" s="4"/>
       <c r="F1" s="4"/>
     </row>
-    <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:6">
       <c r="A2" s="5" t="s">
         <v>1</v>
       </c>
@@ -973,88 +1187,87 @@
         <v>4</v>
       </c>
       <c r="E2" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="F2" s="8" t="n">
-        <f aca="false">SUM(C3:C99)</f>
+        <v>42</v>
+      </c>
+      <c r="F2" s="8">
+        <f>SUM(C3:C99)</f>
         <v>0</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:6">
       <c r="E3" s="4"/>
       <c r="F3" s="4"/>
     </row>
-    <row r="4" customFormat="false" ht="58.2" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="4" spans="1:6" ht="51">
       <c r="A4" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B4" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B4" s="2" t="s">
+      <c r="C4" s="9"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1" t="s">
         <v>45</v>
       </c>
-      <c r="C4" s="9"/>
-    </row>
-    <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="1" t="s">
+      <c r="B5" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B5" s="2" t="s">
+      <c r="C5" s="9"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="1" t="s">
         <v>47</v>
       </c>
-      <c r="C5" s="9"/>
-    </row>
-    <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="1" t="s">
+      <c r="B6" s="2" t="s">
+        <v>46</v>
+      </c>
+      <c r="C6" s="9"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="C7" s="9"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="C8" s="9"/>
+    </row>
+    <row r="9" spans="1:6">
+      <c r="C9" s="9"/>
+    </row>
+    <row r="10" spans="1:6">
+      <c r="A10" s="1" t="s">
         <v>48</v>
       </c>
-      <c r="B6" s="2" t="s">
-        <v>47</v>
-      </c>
-      <c r="C6" s="9"/>
-    </row>
-    <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C7" s="9"/>
-    </row>
-    <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C8" s="9"/>
-    </row>
-    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C9" s="9"/>
-    </row>
-    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="1" t="s">
-        <v>49</v>
-      </c>
       <c r="C10" s="9"/>
     </row>
-    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="11" spans="1:6">
       <c r="A11" s="11"/>
       <c r="B11" s="11"/>
     </row>
-    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="12" spans="1:6">
       <c r="A12" s="11"/>
       <c r="B12" s="11"/>
     </row>
-    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:6">
       <c r="A13" s="11"/>
       <c r="B13" s="11"/>
     </row>
-    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="14" spans="1:6">
       <c r="A14" s="11"/>
       <c r="B14" s="11"/>
     </row>
-    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="15" spans="1:6">
       <c r="A15" s="11"/>
       <c r="B15" s="11"/>
     </row>
-    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="16" spans="1:6">
       <c r="A16" s="11"/>
       <c r="B16" s="11"/>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>
@@ -1063,18 +1276,15 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <sheetPr filterMode="false">
-    <pageSetUpPr fitToPage="false"/>
-  </sheetPr>
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="B9" activeCellId="0" sqref="B9"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="B9" sqref="B9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.75"/>
   <sheetData>
-    <row r="1" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" spans="1:2" ht="38.25">
       <c r="A1" s="1" t="s">
         <v>31</v>
       </c>
@@ -1082,7 +1292,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="2" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="2" spans="1:2" ht="38.25">
       <c r="A2" s="1" t="s">
         <v>34</v>
       </c>
@@ -1090,7 +1300,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="3" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="3" spans="1:2" ht="38.25">
       <c r="A3" s="1" t="s">
         <v>37</v>
       </c>
@@ -1098,7 +1308,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="7" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="7" spans="1:2" ht="38.25">
       <c r="A7" s="1" t="s">
         <v>31</v>
       </c>
@@ -1106,7 +1316,7 @@
         <v>32</v>
       </c>
     </row>
-    <row r="8" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="8" spans="1:2" ht="38.25">
       <c r="A8" s="1" t="s">
         <v>34</v>
       </c>
@@ -1114,7 +1324,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="9" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="9" spans="1:2" ht="38.25">
       <c r="A9" s="1" t="s">
         <v>37</v>
       </c>
@@ -1122,35 +1332,34 @@
         <v>38</v>
       </c>
     </row>
-    <row r="13" customFormat="false" ht="252.6" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="13" spans="1:2" ht="280.5">
       <c r="A13" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="B13" s="2" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="2" t="s">
+    </row>
+    <row r="14" spans="1:2" ht="38.25">
+      <c r="A14" s="1" t="s">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="1" t="s">
+      <c r="B14" s="2" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="2" t="s">
+    </row>
+    <row r="15" spans="1:2" ht="38.25">
+      <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="35.4" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="1" t="s">
-        <v>48</v>
-      </c>
       <c r="B15" s="2" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>
-  <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
-  <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="0" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
-  <headerFooter differentFirst="false" differentOddEven="false">
+  <pageMargins left="0.78749999999999998" right="0.78749999999999998" top="1.05277777777778" bottom="1.05277777777778" header="0.78749999999999998" footer="0.78749999999999998"/>
+  <pageSetup firstPageNumber="0" orientation="portrait" horizontalDpi="300" verticalDpi="300"/>
+  <headerFooter>
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
   </headerFooter>

</xml_diff>